<commit_message>
GPU and PortID support
- separated rv and psm3 into different INSTALL components
- improved to support GPU
- improved to get port number from port id (port name)
- improved CLI command input and output to support port id
- improved to support impi installed from Intel oneAPI

Signed-off-by: Wang, Jijun <jijun.wang@intel.com>
</commit_message>
<xml_diff>
--- a/IbaTools/ethxlattopology/detailed_topology.xlsx
+++ b/IbaTools/ethxlattopology/detailed_topology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jijunwan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C091ED-45E2-4B70-903E-3696C4FCAD73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600544E-CD12-46B6-955F-2EE5644C4DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7365" yWindow="1065" windowWidth="19305" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fabric Links" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7496" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7513" uniqueCount="246">
   <si>
     <t>1m</t>
   </si>
@@ -780,6 +780,33 @@
   </si>
   <si>
     <t>SWD24</t>
+  </si>
+  <si>
+    <t>Eth1/19</t>
+  </si>
+  <si>
+    <t>Eth1/20</t>
+  </si>
+  <si>
+    <t>Eth1/21</t>
+  </si>
+  <si>
+    <t>Eth1/22</t>
+  </si>
+  <si>
+    <t>Eth1/1</t>
+  </si>
+  <si>
+    <t>Eth1/2</t>
+  </si>
+  <si>
+    <t>Eth1/3</t>
+  </si>
+  <si>
+    <t>Eth1/4</t>
+  </si>
+  <si>
+    <t>Eth1</t>
   </si>
 </sst>
 </file>
@@ -1812,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,8 +1982,8 @@
         <v>178</v>
       </c>
       <c r="J4" s="7"/>
-      <c r="K4" s="7">
-        <v>1</v>
+      <c r="K4" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>15</v>
@@ -1993,8 +2020,8 @@
         <v>180</v>
       </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="7">
-        <v>2</v>
+      <c r="K5" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="5" t="s">
@@ -2029,8 +2056,8 @@
         <v>182</v>
       </c>
       <c r="J6" s="7"/>
-      <c r="K6" s="7">
-        <v>3</v>
+      <c r="K6" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="5" t="s">
@@ -2065,8 +2092,8 @@
         <v>184</v>
       </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="7">
-        <v>4</v>
+      <c r="K7" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="5" t="s">
@@ -2257,8 +2284,8 @@
         <v>178</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="6">
-        <v>19</v>
+      <c r="E12" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>15</v>
@@ -2303,8 +2330,8 @@
         <v>180</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="6">
-        <v>20</v>
+      <c r="E13" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="5"/>
@@ -2343,8 +2370,8 @@
         <v>182</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="6">
-        <v>21</v>
+      <c r="E14" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="5"/>
@@ -2383,8 +2410,8 @@
         <v>184</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="6">
-        <v>22</v>
+      <c r="E15" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="5"/>
@@ -2445,8 +2472,8 @@
         <v>186</v>
       </c>
       <c r="J16" s="7"/>
-      <c r="K16" s="7">
-        <v>1</v>
+      <c r="K16" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>15</v>
@@ -2483,8 +2510,8 @@
         <v>188</v>
       </c>
       <c r="J17" s="7"/>
-      <c r="K17" s="7">
-        <v>2</v>
+      <c r="K17" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="5" t="s">
@@ -2519,8 +2546,8 @@
         <v>190</v>
       </c>
       <c r="J18" s="7"/>
-      <c r="K18" s="7">
-        <v>3</v>
+      <c r="K18" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="5" t="s">
@@ -2555,8 +2582,8 @@
         <v>192</v>
       </c>
       <c r="J19" s="7"/>
-      <c r="K19" s="7">
-        <v>4</v>
+      <c r="K19" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="5" t="s">
@@ -2747,8 +2774,8 @@
         <v>186</v>
       </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="6">
-        <v>19</v>
+      <c r="E24" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>15</v>
@@ -2793,8 +2820,8 @@
         <v>188</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="6">
-        <v>20</v>
+      <c r="E25" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5"/>
@@ -2833,8 +2860,8 @@
         <v>190</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="6">
-        <v>21</v>
+      <c r="E26" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
@@ -2873,8 +2900,8 @@
         <v>192</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="E27" s="6">
-        <v>22</v>
+      <c r="E27" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5"/>
@@ -2933,8 +2960,8 @@
         <v>53</v>
       </c>
       <c r="J28" s="7"/>
-      <c r="K28" s="7">
-        <v>1</v>
+      <c r="K28" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>15</v>
@@ -3075,8 +3102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O293"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView topLeftCell="A199" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10534,7 +10561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O1157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+    <sheetView topLeftCell="A79" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>

</xml_diff>